<commit_message>
created readme and a few changes for usability
</commit_message>
<xml_diff>
--- a/EandD.xlsx
+++ b/EandD.xlsx
@@ -72,9 +72,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="[$-409]h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="168" formatCode="0.000%"/>
-    <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -100,12 +100,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -157,12 +163,12 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -171,42 +177,48 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -527,7 +539,7 @@
   <dimension ref="A1:M151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +547,7 @@
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" customWidth="1"/>
     <col min="3" max="5" width="9" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="20"/>
+    <col min="6" max="6" width="9.140625" style="15"/>
     <col min="7" max="7" width="15.28515625" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" customWidth="1"/>
@@ -544,28 +556,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="20">
+      <c r="I1" s="15">
         <f>F2*1.5</f>
         <v>3474</v>
       </c>
@@ -579,7 +591,7 @@
         <v>193</v>
       </c>
       <c r="B2">
-        <f>SUM($A$2:A2)</f>
+        <f>IF(ISBLANK(A2),"",SUM($A$2:A2))</f>
         <v>193</v>
       </c>
       <c r="C2" s="2">
@@ -588,556 +600,688 @@
       <c r="D2" s="2">
         <v>8.6805555555555566E-2</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="13">
         <f t="shared" ref="E2:E3" si="0">IF(ISBLANK(D2),"",D2-C2)</f>
         <v>3.4722222222222376E-3</v>
       </c>
-      <c r="F2" s="20">
+      <c r="F2" s="15">
         <f>IF(ISBLANK(A2),"",A2/(HOUR(E2) + MINUTE(E2) / 60))</f>
         <v>2316</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="8">
         <f>LOOKUP(2,1/(F:F&lt;&gt;""),F:F)/I1</f>
         <v>0.82243605559667743</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="16">
         <f>1-I2</f>
         <v>0.17756394440332257</v>
       </c>
-      <c r="M2" s="11"/>
+      <c r="M2" s="17"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5000</v>
       </c>
+      <c r="B3">
+        <f>IF(ISBLANK(A3),"",SUM($A$2:A3))</f>
+        <v>5193</v>
+      </c>
       <c r="C3" s="2">
         <v>0.16666666666666666</v>
       </c>
       <c r="D3" s="2">
         <v>0.23958333333333334</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="13">
         <f t="shared" si="0"/>
         <v>7.2916666666666685E-2</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="15">
         <f t="shared" ref="F3:F11" si="1">IF(ISBLANK(A3),"",A3/(HOUR(E3) + MINUTE(E3) / 60))</f>
         <v>2857.1428571428573</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="17" t="str">
+      <c r="B4" t="str">
+        <f>IF(ISBLANK(A4),"",SUM($A$2:A4))</f>
+        <v/>
+      </c>
+      <c r="E4" s="13" t="str">
         <f>IF(ISBLANK(D4),"",D4-C4)</f>
         <v/>
       </c>
-      <c r="F4" s="20" t="str">
+      <c r="F4" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="22">
         <v>70000</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="6"/>
+      <c r="M4" s="19"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="17" t="str">
+      <c r="B5" t="str">
+        <f>IF(ISBLANK(A5),"",SUM($A$2:A5))</f>
+        <v/>
+      </c>
+      <c r="E5" s="13" t="str">
         <f t="shared" ref="E5:E27" si="2">IF(ISBLANK(D5),"",D5-C5)</f>
         <v/>
       </c>
-      <c r="F5" s="20" t="str">
+      <c r="F5" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="7">
         <f>SUM(A:A)/I4</f>
         <v>7.4185714285714285E-2</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="16">
         <f>1-I5</f>
         <v>0.9258142857142857</v>
       </c>
-      <c r="M5" s="11"/>
+      <c r="M5" s="17"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E6" s="17" t="str">
+      <c r="B6" t="str">
+        <f>IF(ISBLANK(A6),"",SUM($A$2:A6))</f>
+        <v/>
+      </c>
+      <c r="E6" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F6" s="20" t="str">
+      <c r="F6" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E7" s="17" t="str">
+      <c r="B7" t="str">
+        <f>IF(ISBLANK(A7),"",SUM($A$2:A7))</f>
+        <v/>
+      </c>
+      <c r="E7" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F7" s="20" t="str">
+      <c r="F7" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E8" s="17" t="str">
+      <c r="B8" t="str">
+        <f>IF(ISBLANK(A8),"",SUM($A$2:A8))</f>
+        <v/>
+      </c>
+      <c r="E8" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F8" s="20" t="str">
+      <c r="F8" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E9" s="17" t="str">
+      <c r="B9" t="str">
+        <f>IF(ISBLANK(A9),"",SUM($A$2:A9))</f>
+        <v/>
+      </c>
+      <c r="E9" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F9" s="20" t="str">
+      <c r="F9" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="H9" s="12" t="str">
+      <c r="H9" s="9" t="str">
         <f>IF(COUNTIF(A:A,"&gt;=5000")&gt;0,"Wrote over 5,000 words in one sprint!","Achievement Locked")</f>
         <v>Wrote over 5,000 words in one sprint!</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E10" s="17" t="str">
+      <c r="B10" t="str">
+        <f>IF(ISBLANK(A10),"",SUM($A$2:A10))</f>
+        <v/>
+      </c>
+      <c r="E10" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F10" s="20" t="str">
+      <c r="F10" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="H10" s="12" t="str">
+      <c r="H10" s="9" t="str">
         <f>IF(COUNTIF(E:E,"&gt;"&amp;TIME(0,30,0)),"Wrote for over 30 minutes!","Achievement Locked")</f>
         <v>Wrote for over 30 minutes!</v>
       </c>
-      <c r="M10" s="16"/>
+      <c r="M10" s="12"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E11" s="17" t="str">
+      <c r="B11" t="str">
+        <f>IF(ISBLANK(A11),"",SUM($A$2:A11))</f>
+        <v/>
+      </c>
+      <c r="E11" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F11" s="20" t="str">
+      <c r="F11" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="G11">
-        <f>COUNTIF(F:F,"&gt;I2")</f>
-        <v>1</v>
-      </c>
-      <c r="H11" s="12" t="str">
-        <f>IF(COUNTIF(F:F,"&gt;I1")&gt;0,"Killed a Minion!","Achievement Locked")</f>
+      <c r="H11" s="9" t="str">
+        <f>IF(COUNTIF(F:F,"&gt;i2")&gt;0,"Killed a Minion!","Achievement Locked")</f>
         <v>Killed a Minion!</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E12" s="17" t="str">
+      <c r="B12" t="str">
+        <f>IF(ISBLANK(A12),"",SUM($A$2:A12))</f>
+        <v/>
+      </c>
+      <c r="E12" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F12" s="20" t="str">
-        <f t="shared" ref="F3:F66" si="3">IF(ISBLANK(A12),"",A12/(HOUR(E12) + MINUTE(E12) / 60))</f>
-        <v/>
-      </c>
-      <c r="H12" s="12" t="str">
-        <f t="shared" ref="H10:H16" si="4">IF(COUNTIF(A:A,"&gt;=5000")&gt;0,"Wrote over 5,000 words in one sprint!","Achievement Locked")</f>
-        <v>Wrote over 5,000 words in one sprint!</v>
+      <c r="F12" s="15" t="str">
+        <f t="shared" ref="F12:F66" si="3">IF(ISBLANK(A12),"",A12/(HOUR(E12) + MINUTE(E12) / 60))</f>
+        <v/>
+      </c>
+      <c r="H12" s="9" t="str">
+        <f>IF(COUNTIF(A:A,"&gt;=50000")&gt;0,"Wrote over 5,000 words in one sprint!","Achievement Locked")</f>
+        <v>Achievement Locked</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E13" s="17" t="str">
+      <c r="B13" t="str">
+        <f>IF(ISBLANK(A13),"",SUM($A$2:A13))</f>
+        <v/>
+      </c>
+      <c r="E13" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F13" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H13" s="12" t="str">
+      <c r="F13" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H13" s="9" t="str">
+        <f t="shared" ref="H13:H16" si="4">IF(COUNTIF(A:A,"&gt;=50000")&gt;0,"Wrote over 5,000 words in one sprint!","Achievement Locked")</f>
+        <v>Achievement Locked</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" t="str">
+        <f>IF(ISBLANK(A14),"",SUM($A$2:A14))</f>
+        <v/>
+      </c>
+      <c r="E14" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="F14" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H14" s="9" t="str">
         <f t="shared" si="4"/>
-        <v>Wrote over 5,000 words in one sprint!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E14" s="17" t="str">
+        <v>Achievement Locked</v>
+      </c>
+      <c r="J14" s="11"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" t="str">
+        <f>IF(ISBLANK(A15),"",SUM($A$2:A15))</f>
+        <v/>
+      </c>
+      <c r="E15" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F14" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H14" s="12" t="str">
+      <c r="F15" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H15" s="9" t="str">
         <f t="shared" si="4"/>
-        <v>Wrote over 5,000 words in one sprint!</v>
-      </c>
-      <c r="J14" s="15"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E15" s="17" t="str">
+        <v>Achievement Locked</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" t="str">
+        <f>IF(ISBLANK(A16),"",SUM($A$2:A16))</f>
+        <v/>
+      </c>
+      <c r="E16" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F15" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H15" s="12" t="str">
+      <c r="F16" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H16" s="9" t="str">
         <f t="shared" si="4"/>
-        <v>Wrote over 5,000 words in one sprint!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E16" s="17" t="str">
+        <v>Achievement Locked</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="str">
+        <f>IF(ISBLANK(A17),"",SUM($A$2:A17))</f>
+        <v/>
+      </c>
+      <c r="E17" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F16" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H16" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v>Wrote over 5,000 words in one sprint!</v>
-      </c>
-    </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E17" s="17" t="str">
+      <c r="F17" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="str">
+        <f>IF(ISBLANK(A18),"",SUM($A$2:A18))</f>
+        <v/>
+      </c>
+      <c r="E18" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F17" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E18" s="17" t="str">
+      <c r="F18" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="str">
+        <f>IF(ISBLANK(A19),"",SUM($A$2:A19))</f>
+        <v/>
+      </c>
+      <c r="E19" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F18" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E19" s="17" t="str">
+      <c r="F19" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="str">
+        <f>IF(ISBLANK(A20),"",SUM($A$2:A20))</f>
+        <v/>
+      </c>
+      <c r="E20" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F19" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E20" s="17" t="str">
+      <c r="F20" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" t="str">
+        <f>IF(ISBLANK(A21),"",SUM($A$2:A21))</f>
+        <v/>
+      </c>
+      <c r="E21" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F20" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E21" s="17" t="str">
+      <c r="F21" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="str">
+        <f>IF(ISBLANK(A22),"",SUM($A$2:A22))</f>
+        <v/>
+      </c>
+      <c r="E22" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F21" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E22" s="17" t="str">
+      <c r="F22" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" t="str">
+        <f>IF(ISBLANK(A23),"",SUM($A$2:A23))</f>
+        <v/>
+      </c>
+      <c r="E23" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F22" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E23" s="17" t="str">
+      <c r="F23" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" t="str">
+        <f>IF(ISBLANK(A24),"",SUM($A$2:A24))</f>
+        <v/>
+      </c>
+      <c r="E24" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F23" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E24" s="17" t="str">
+      <c r="F24" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="str">
+        <f>IF(ISBLANK(A25),"",SUM($A$2:A25))</f>
+        <v/>
+      </c>
+      <c r="E25" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F24" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E25" s="17" t="str">
+      <c r="F25" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" t="str">
+        <f>IF(ISBLANK(A26),"",SUM($A$2:A26))</f>
+        <v/>
+      </c>
+      <c r="E26" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F25" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E26" s="17" t="str">
+      <c r="F26" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" t="str">
+        <f>IF(ISBLANK(A27),"",SUM($A$2:A27))</f>
+        <v/>
+      </c>
+      <c r="E27" s="13" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F26" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E27" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="F27" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F27" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" t="str">
+        <f>IF(ISBLANK(A28),"",SUM($A$2:A28))</f>
+        <v/>
+      </c>
       <c r="E28" s="3" t="str">
-        <f t="shared" ref="E3:E66" si="5">IF(ISBLANK(D28),"",TEXT(D28-C28, "h:mm"))</f>
-        <v/>
-      </c>
-      <c r="F28" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="5:8" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E28:E66" si="5">IF(ISBLANK(D28),"",TEXT(D28-C28, "h:mm"))</f>
+        <v/>
+      </c>
+      <c r="F28" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" t="str">
+        <f>IF(ISBLANK(A29),"",SUM($A$2:A29))</f>
+        <v/>
+      </c>
       <c r="E29" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F29" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F29" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" t="str">
+        <f>IF(ISBLANK(A30),"",SUM($A$2:A30))</f>
+        <v/>
+      </c>
       <c r="E30" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F30" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F30" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" t="str">
+        <f>IF(ISBLANK(A31),"",SUM($A$2:A31))</f>
+        <v/>
+      </c>
       <c r="E31" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F31" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F31" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" t="str">
+        <f>IF(ISBLANK(A32),"",SUM($A$2:A32))</f>
+        <v/>
+      </c>
       <c r="E32" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F32" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" t="str">
+        <f>IF(ISBLANK(A33),"",SUM($A$2:A33))</f>
+        <v/>
+      </c>
       <c r="E33" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F33" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="str">
+        <f>IF(ISBLANK(A34),"",SUM($A$2:A34))</f>
+        <v/>
+      </c>
       <c r="E34" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F34" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="str">
+        <f>IF(ISBLANK(A35),"",SUM($A$2:A35))</f>
+        <v/>
+      </c>
       <c r="E35" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F35" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" t="str">
+        <f>IF(ISBLANK(A36),"",SUM($A$2:A36))</f>
+        <v/>
+      </c>
       <c r="E36" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F36" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E37" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F37" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E38" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F38" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E39" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F39" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E40" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F40" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E41" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F41" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F41" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E42" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F42" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E43" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F43" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F43" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E44" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F44" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F44" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E45" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F45" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F45" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E46" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F46" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F46" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E47" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F47" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F47" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E48" s="3" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F48" s="20" t="str">
+      <c r="F48" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1147,7 +1291,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F49" s="20" t="str">
+      <c r="F49" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1157,7 +1301,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F50" s="20" t="str">
+      <c r="F50" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1167,7 +1311,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F51" s="20" t="str">
+      <c r="F51" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1177,7 +1321,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F52" s="20" t="str">
+      <c r="F52" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1187,7 +1331,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F53" s="20" t="str">
+      <c r="F53" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1197,7 +1341,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F54" s="20" t="str">
+      <c r="F54" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1207,7 +1351,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F55" s="20" t="str">
+      <c r="F55" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1217,7 +1361,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F56" s="20" t="str">
+      <c r="F56" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1227,7 +1371,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F57" s="20" t="str">
+      <c r="F57" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1237,7 +1381,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F58" s="20" t="str">
+      <c r="F58" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1247,7 +1391,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F59" s="20" t="str">
+      <c r="F59" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1257,7 +1401,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F60" s="20" t="str">
+      <c r="F60" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1267,7 +1411,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F61" s="20" t="str">
+      <c r="F61" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1277,7 +1421,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F62" s="20" t="str">
+      <c r="F62" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1287,7 +1431,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F63" s="20" t="str">
+      <c r="F63" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1297,7 +1441,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F64" s="20" t="str">
+      <c r="F64" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1307,7 +1451,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F65" s="20" t="str">
+      <c r="F65" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1317,7 +1461,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F66" s="20" t="str">
+      <c r="F66" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1327,7 +1471,7 @@
         <f t="shared" ref="E67:E130" si="6">IF(ISBLANK(D67),"",TEXT(D67-C67, "h:mm"))</f>
         <v/>
       </c>
-      <c r="F67" s="20" t="str">
+      <c r="F67" s="15" t="str">
         <f t="shared" ref="F67:F81" si="7">IF(ISBLANK(A67),"",A67/(HOUR(E67) + MINUTE(E67) / 60))</f>
         <v/>
       </c>
@@ -1337,7 +1481,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F68" s="20" t="str">
+      <c r="F68" s="15" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -1347,7 +1491,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F69" s="20" t="str">
+      <c r="F69" s="15" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -1357,7 +1501,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F70" s="20" t="str">
+      <c r="F70" s="15" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -1367,7 +1511,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F71" s="20" t="str">
+      <c r="F71" s="15" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -1377,7 +1521,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F72" s="20" t="str">
+      <c r="F72" s="15" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -1387,7 +1531,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F73" s="20" t="str">
+      <c r="F73" s="15" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -1397,7 +1541,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F74" s="20" t="str">
+      <c r="F74" s="15" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -1407,7 +1551,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F75" s="20" t="str">
+      <c r="F75" s="15" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -1417,7 +1561,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F76" s="20" t="str">
+      <c r="F76" s="15" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -1427,7 +1571,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F77" s="20" t="str">
+      <c r="F77" s="15" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -1437,7 +1581,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F78" s="20" t="str">
+      <c r="F78" s="15" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -1447,7 +1591,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F79" s="20" t="str">
+      <c r="F79" s="15" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -1457,7 +1601,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F80" s="20" t="str">
+      <c r="F80" s="15" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -1467,7 +1611,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F81" s="20" t="str">
+      <c r="F81" s="15" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
@@ -1477,8 +1621,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F82" s="20" t="str">
-        <f t="shared" ref="F68:F121" si="8">IF(ISBLANK(A82),"",A82/(HOUR(E82) + MINUTE(E82) / 60))</f>
+      <c r="F82" s="15" t="str">
+        <f t="shared" ref="F82:F121" si="8">IF(ISBLANK(A82),"",A82/(HOUR(E82) + MINUTE(E82) / 60))</f>
         <v/>
       </c>
     </row>
@@ -1487,7 +1631,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F83" s="20" t="str">
+      <c r="F83" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1497,7 +1641,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F84" s="20" t="str">
+      <c r="F84" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1507,7 +1651,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F85" s="20" t="str">
+      <c r="F85" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1517,7 +1661,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F86" s="20" t="str">
+      <c r="F86" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1527,7 +1671,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F87" s="20" t="str">
+      <c r="F87" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1537,7 +1681,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F88" s="20" t="str">
+      <c r="F88" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1547,7 +1691,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F89" s="20" t="str">
+      <c r="F89" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1557,7 +1701,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F90" s="20" t="str">
+      <c r="F90" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1567,7 +1711,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F91" s="20" t="str">
+      <c r="F91" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1577,7 +1721,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F92" s="20" t="str">
+      <c r="F92" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1587,7 +1731,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F93" s="20" t="str">
+      <c r="F93" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1597,7 +1741,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F94" s="20" t="str">
+      <c r="F94" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1607,7 +1751,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F95" s="20" t="str">
+      <c r="F95" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1617,7 +1761,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F96" s="20" t="str">
+      <c r="F96" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1627,7 +1771,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F97" s="20" t="str">
+      <c r="F97" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1637,7 +1781,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F98" s="20" t="str">
+      <c r="F98" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1647,7 +1791,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F99" s="20" t="str">
+      <c r="F99" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1657,7 +1801,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F100" s="20" t="str">
+      <c r="F100" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1667,7 +1811,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F101" s="20" t="str">
+      <c r="F101" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1677,7 +1821,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F102" s="20" t="str">
+      <c r="F102" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1687,7 +1831,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F103" s="20" t="str">
+      <c r="F103" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1697,7 +1841,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F104" s="20" t="str">
+      <c r="F104" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1707,7 +1851,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F105" s="20" t="str">
+      <c r="F105" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1717,7 +1861,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F106" s="20" t="str">
+      <c r="F106" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1727,7 +1871,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F107" s="20" t="str">
+      <c r="F107" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1737,7 +1881,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F108" s="20" t="str">
+      <c r="F108" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1747,7 +1891,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F109" s="20" t="str">
+      <c r="F109" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1757,7 +1901,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F110" s="20" t="str">
+      <c r="F110" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1767,7 +1911,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F111" s="20" t="str">
+      <c r="F111" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1777,7 +1921,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F112" s="20" t="str">
+      <c r="F112" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1787,7 +1931,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F113" s="20" t="str">
+      <c r="F113" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1797,7 +1941,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F114" s="20" t="str">
+      <c r="F114" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1807,7 +1951,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F115" s="20" t="str">
+      <c r="F115" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1817,7 +1961,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F116" s="20" t="str">
+      <c r="F116" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1827,7 +1971,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F117" s="20" t="str">
+      <c r="F117" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1837,7 +1981,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F118" s="20" t="str">
+      <c r="F118" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1847,7 +1991,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F119" s="20" t="str">
+      <c r="F119" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1857,7 +2001,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F120" s="20" t="str">
+      <c r="F120" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -1867,7 +2011,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="F121" s="20" t="str">
+      <c r="F121" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>

</xml_diff>

<commit_message>
updated achievements and fixed minion death formula
</commit_message>
<xml_diff>
--- a/EandD.xlsx
+++ b/EandD.xlsx
@@ -163,7 +163,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -185,9 +185,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -200,6 +197,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -212,13 +216,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -539,7 +538,7 @@
   <dimension ref="A1:M151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,7 +546,7 @@
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" customWidth="1"/>
     <col min="3" max="5" width="9" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="15"/>
+    <col min="6" max="6" width="9.140625" style="14"/>
     <col min="7" max="7" width="15.28515625" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" customWidth="1"/>
@@ -556,35 +555,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="15">
+      <c r="I1" s="14">
         <f>F2*1.5</f>
         <v>3474</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="18"/>
+      <c r="M1" s="20"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -600,11 +599,11 @@
       <c r="D2" s="2">
         <v>8.6805555555555566E-2</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="12">
         <f t="shared" ref="E2:E3" si="0">IF(ISBLANK(D2),"",D2-C2)</f>
         <v>3.4722222222222376E-3</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="14">
         <f>IF(ISBLANK(A2),"",A2/(HOUR(E2) + MINUTE(E2) / 60))</f>
         <v>2316</v>
       </c>
@@ -615,11 +614,11 @@
         <f>LOOKUP(2,1/(F:F&lt;&gt;""),F:F)/I1</f>
         <v>0.82243605559667743</v>
       </c>
-      <c r="L2" s="16">
+      <c r="L2" s="18">
         <f>1-I2</f>
         <v>0.17756394440332257</v>
       </c>
-      <c r="M2" s="17"/>
+      <c r="M2" s="19"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -635,11 +634,11 @@
       <c r="D3" s="2">
         <v>0.23958333333333334</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="12">
         <f t="shared" si="0"/>
         <v>7.2916666666666685E-2</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="14">
         <f t="shared" ref="F3:F11" si="1">IF(ISBLANK(A3),"",A3/(HOUR(E3) + MINUTE(E3) / 60))</f>
         <v>2857.1428571428573</v>
       </c>
@@ -649,35 +648,35 @@
         <f>IF(ISBLANK(A4),"",SUM($A$2:A4))</f>
         <v/>
       </c>
-      <c r="E4" s="13" t="str">
+      <c r="E4" s="12" t="str">
         <f>IF(ISBLANK(D4),"",D4-C4)</f>
         <v/>
       </c>
-      <c r="F4" s="15" t="str">
+      <c r="F4" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="22">
+      <c r="I4" s="17">
         <v>70000</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="19"/>
+      <c r="M4" s="21"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" t="str">
         <f>IF(ISBLANK(A5),"",SUM($A$2:A5))</f>
         <v/>
       </c>
-      <c r="E5" s="13" t="str">
+      <c r="E5" s="12" t="str">
         <f t="shared" ref="E5:E27" si="2">IF(ISBLANK(D5),"",D5-C5)</f>
         <v/>
       </c>
-      <c r="F5" s="15" t="str">
+      <c r="F5" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -688,22 +687,22 @@
         <f>SUM(A:A)/I4</f>
         <v>7.4185714285714285E-2</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="18">
         <f>1-I5</f>
         <v>0.9258142857142857</v>
       </c>
-      <c r="M5" s="17"/>
+      <c r="M5" s="19"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="str">
         <f>IF(ISBLANK(A6),"",SUM($A$2:A6))</f>
         <v/>
       </c>
-      <c r="E6" s="13" t="str">
+      <c r="E6" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F6" s="15" t="str">
+      <c r="F6" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -713,11 +712,11 @@
         <f>IF(ISBLANK(A7),"",SUM($A$2:A7))</f>
         <v/>
       </c>
-      <c r="E7" s="13" t="str">
+      <c r="E7" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F7" s="15" t="str">
+      <c r="F7" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -727,15 +726,15 @@
         <f>IF(ISBLANK(A8),"",SUM($A$2:A8))</f>
         <v/>
       </c>
-      <c r="E8" s="13" t="str">
+      <c r="E8" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F8" s="15" t="str">
+      <c r="F8" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -744,15 +743,15 @@
         <f>IF(ISBLANK(A9),"",SUM($A$2:A9))</f>
         <v/>
       </c>
-      <c r="E9" s="13" t="str">
+      <c r="E9" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F9" s="15" t="str">
+      <c r="F9" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="H9" s="9" t="str">
+      <c r="H9" s="23" t="str">
         <f>IF(COUNTIF(A:A,"&gt;=5000")&gt;0,"Wrote over 5,000 words in one sprint!","Achievement Locked")</f>
         <v>Wrote over 5,000 words in one sprint!</v>
       </c>
@@ -762,36 +761,36 @@
         <f>IF(ISBLANK(A10),"",SUM($A$2:A10))</f>
         <v/>
       </c>
-      <c r="E10" s="13" t="str">
+      <c r="E10" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F10" s="15" t="str">
+      <c r="F10" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="H10" s="9" t="str">
+      <c r="H10" s="23" t="str">
         <f>IF(COUNTIF(E:E,"&gt;"&amp;TIME(0,30,0)),"Wrote for over 30 minutes!","Achievement Locked")</f>
         <v>Wrote for over 30 minutes!</v>
       </c>
-      <c r="M10" s="12"/>
+      <c r="M10" s="11"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <f>IF(ISBLANK(A11),"",SUM($A$2:A11))</f>
         <v/>
       </c>
-      <c r="E11" s="13" t="str">
+      <c r="E11" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F11" s="15" t="str">
+      <c r="F11" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="H11" s="9" t="str">
-        <f>IF(COUNTIF(F:F,"&gt;i2")&gt;0,"Killed a Minion!","Achievement Locked")</f>
-        <v>Killed a Minion!</v>
+      <c r="H11" s="23" t="str">
+        <f>IF(COUNTIF(F:F,"&gt;"&amp;I1)&gt;0,"Killed a Minion!","Achievement Locked")</f>
+        <v>Achievement Locked</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -799,16 +798,16 @@
         <f>IF(ISBLANK(A12),"",SUM($A$2:A12))</f>
         <v/>
       </c>
-      <c r="E12" s="13" t="str">
+      <c r="E12" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F12" s="15" t="str">
+      <c r="F12" s="14" t="str">
         <f t="shared" ref="F12:F66" si="3">IF(ISBLANK(A12),"",A12/(HOUR(E12) + MINUTE(E12) / 60))</f>
         <v/>
       </c>
-      <c r="H12" s="9" t="str">
-        <f>IF(COUNTIF(A:A,"&gt;=50000")&gt;0,"Wrote over 5,000 words in one sprint!","Achievement Locked")</f>
+      <c r="H12" s="23" t="str">
+        <f>IF(COUNTIF(A:A,"&gt;=1")&gt;5,"Logged 5 Writing Sprints!","Achievement Locked")</f>
         <v>Achievement Locked</v>
       </c>
     </row>
@@ -817,16 +816,16 @@
         <f>IF(ISBLANK(A13),"",SUM($A$2:A13))</f>
         <v/>
       </c>
-      <c r="E13" s="13" t="str">
+      <c r="E13" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F13" s="15" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H13" s="9" t="str">
-        <f t="shared" ref="H13:H16" si="4">IF(COUNTIF(A:A,"&gt;=50000")&gt;0,"Wrote over 5,000 words in one sprint!","Achievement Locked")</f>
+      <c r="F13" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H13" s="23" t="str">
+        <f>IF(COUNTIF(A:A,"&gt;=1")&gt;15,"Logged 15 Writing Sprints!","Achievement Locked")</f>
         <v>Achievement Locked</v>
       </c>
     </row>
@@ -835,35 +834,35 @@
         <f>IF(ISBLANK(A14),"",SUM($A$2:A14))</f>
         <v/>
       </c>
-      <c r="E14" s="13" t="str">
+      <c r="E14" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F14" s="15" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H14" s="9" t="str">
-        <f t="shared" si="4"/>
+      <c r="F14" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H14" s="23" t="str">
+        <f>IF(COUNTIF(A:A,"&gt;=1")&gt;50,"Logged 50 Writing Sprints! YOU MACHINE","Achievement Locked")</f>
         <v>Achievement Locked</v>
       </c>
-      <c r="J14" s="11"/>
+      <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <f>IF(ISBLANK(A15),"",SUM($A$2:A15))</f>
         <v/>
       </c>
-      <c r="E15" s="13" t="str">
+      <c r="E15" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F15" s="15" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H15" s="9" t="str">
-        <f t="shared" si="4"/>
+      <c r="F15" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H15" s="23" t="str">
+        <f>IF(I5&gt;50%,"Halfway to boss death!","Achievement Locked")</f>
         <v>Achievement Locked</v>
       </c>
     </row>
@@ -872,16 +871,16 @@
         <f>IF(ISBLANK(A16),"",SUM($A$2:A16))</f>
         <v/>
       </c>
-      <c r="E16" s="13" t="str">
+      <c r="E16" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F16" s="15" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H16" s="9" t="str">
-        <f t="shared" si="4"/>
+      <c r="F16" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H16" s="23" t="str">
+        <f>IF(COUNTIF(F:F,"&gt;"&amp;I1*0.9)&gt;0,"Minion barely survived!","Achievement Locked")</f>
         <v>Achievement Locked</v>
       </c>
     </row>
@@ -890,54 +889,59 @@
         <f>IF(ISBLANK(A17),"",SUM($A$2:A17))</f>
         <v/>
       </c>
-      <c r="E17" s="13" t="str">
+      <c r="E17" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F17" s="15" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H17" s="3"/>
+      <c r="F17" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H17" s="22" t="str">
+        <f>IF(I5&gt;100%,"HOLY CRAP YOU KILLED THE BOSS!","Achievement Locked")</f>
+        <v>Achievement Locked</v>
+      </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>IF(ISBLANK(A18),"",SUM($A$2:A18))</f>
         <v/>
       </c>
-      <c r="E18" s="13" t="str">
+      <c r="E18" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F18" s="15" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+      <c r="F18" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H18" s="23"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>IF(ISBLANK(A19),"",SUM($A$2:A19))</f>
         <v/>
       </c>
-      <c r="E19" s="13" t="str">
+      <c r="E19" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F19" s="15" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+      <c r="F19" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H19" s="23"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>IF(ISBLANK(A20),"",SUM($A$2:A20))</f>
         <v/>
       </c>
-      <c r="E20" s="13" t="str">
+      <c r="E20" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F20" s="15" t="str">
+      <c r="F20" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -947,11 +951,11 @@
         <f>IF(ISBLANK(A21),"",SUM($A$2:A21))</f>
         <v/>
       </c>
-      <c r="E21" s="13" t="str">
+      <c r="E21" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F21" s="15" t="str">
+      <c r="F21" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -961,11 +965,11 @@
         <f>IF(ISBLANK(A22),"",SUM($A$2:A22))</f>
         <v/>
       </c>
-      <c r="E22" s="13" t="str">
+      <c r="E22" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F22" s="15" t="str">
+      <c r="F22" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -975,11 +979,11 @@
         <f>IF(ISBLANK(A23),"",SUM($A$2:A23))</f>
         <v/>
       </c>
-      <c r="E23" s="13" t="str">
+      <c r="E23" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F23" s="15" t="str">
+      <c r="F23" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -989,11 +993,11 @@
         <f>IF(ISBLANK(A24),"",SUM($A$2:A24))</f>
         <v/>
       </c>
-      <c r="E24" s="13" t="str">
+      <c r="E24" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F24" s="15" t="str">
+      <c r="F24" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1003,11 +1007,11 @@
         <f>IF(ISBLANK(A25),"",SUM($A$2:A25))</f>
         <v/>
       </c>
-      <c r="E25" s="13" t="str">
+      <c r="E25" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F25" s="15" t="str">
+      <c r="F25" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1017,11 +1021,11 @@
         <f>IF(ISBLANK(A26),"",SUM($A$2:A26))</f>
         <v/>
       </c>
-      <c r="E26" s="13" t="str">
+      <c r="E26" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F26" s="15" t="str">
+      <c r="F26" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1031,11 +1035,11 @@
         <f>IF(ISBLANK(A27),"",SUM($A$2:A27))</f>
         <v/>
       </c>
-      <c r="E27" s="13" t="str">
+      <c r="E27" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F27" s="15" t="str">
+      <c r="F27" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1046,10 +1050,10 @@
         <v/>
       </c>
       <c r="E28" s="3" t="str">
-        <f t="shared" ref="E28:E66" si="5">IF(ISBLANK(D28),"",TEXT(D28-C28, "h:mm"))</f>
-        <v/>
-      </c>
-      <c r="F28" s="15" t="str">
+        <f t="shared" ref="E28:E66" si="4">IF(ISBLANK(D28),"",TEXT(D28-C28, "h:mm"))</f>
+        <v/>
+      </c>
+      <c r="F28" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1060,10 +1064,10 @@
         <v/>
       </c>
       <c r="E29" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F29" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F29" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1074,10 +1078,10 @@
         <v/>
       </c>
       <c r="E30" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F30" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F30" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1088,10 +1092,10 @@
         <v/>
       </c>
       <c r="E31" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F31" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F31" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1102,10 +1106,10 @@
         <v/>
       </c>
       <c r="E32" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F32" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F32" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1116,10 +1120,10 @@
         <v/>
       </c>
       <c r="E33" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F33" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F33" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1130,10 +1134,10 @@
         <v/>
       </c>
       <c r="E34" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F34" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F34" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1144,10 +1148,10 @@
         <v/>
       </c>
       <c r="E35" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F35" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F35" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -1158,1041 +1162,1041 @@
         <v/>
       </c>
       <c r="E36" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F36" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F36" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E37" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F37" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F37" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E38" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F38" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F38" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E39" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F39" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F39" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E40" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F40" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F40" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E41" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F41" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F41" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E42" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F42" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F42" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E43" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F43" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F43" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E44" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F44" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F44" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E45" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F45" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F45" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E46" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F46" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F46" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E47" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F47" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F47" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E48" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F48" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F48" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="49" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E49" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F49" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F49" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="50" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E50" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F50" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F50" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="51" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E51" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F51" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F51" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="52" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E52" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F52" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F52" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="53" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E53" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F53" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F53" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="54" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E54" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F54" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F54" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="55" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E55" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F55" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F55" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="56" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E56" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F56" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F56" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="57" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E57" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F57" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F57" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="58" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E58" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F58" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F58" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="59" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E59" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F59" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F59" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="60" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E60" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F60" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F60" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="61" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E61" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F61" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F61" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="62" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E62" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F62" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F62" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="63" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E63" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F63" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F63" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="64" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E64" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F64" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F64" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="65" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E65" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F65" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F65" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="66" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E66" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F66" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F66" s="14" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="67" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E67" s="3" t="str">
-        <f t="shared" ref="E67:E130" si="6">IF(ISBLANK(D67),"",TEXT(D67-C67, "h:mm"))</f>
-        <v/>
-      </c>
-      <c r="F67" s="15" t="str">
-        <f t="shared" ref="F67:F81" si="7">IF(ISBLANK(A67),"",A67/(HOUR(E67) + MINUTE(E67) / 60))</f>
+        <f t="shared" ref="E67:E130" si="5">IF(ISBLANK(D67),"",TEXT(D67-C67, "h:mm"))</f>
+        <v/>
+      </c>
+      <c r="F67" s="14" t="str">
+        <f t="shared" ref="F67:F81" si="6">IF(ISBLANK(A67),"",A67/(HOUR(E67) + MINUTE(E67) / 60))</f>
         <v/>
       </c>
     </row>
     <row r="68" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E68" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F68" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F68" s="15" t="str">
-        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="69" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E69" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F69" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F69" s="15" t="str">
-        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="70" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E70" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F70" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F70" s="15" t="str">
-        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="71" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E71" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F71" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F71" s="15" t="str">
-        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="72" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E72" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F72" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F72" s="15" t="str">
-        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="73" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E73" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F73" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F73" s="15" t="str">
-        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="74" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E74" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F74" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F74" s="15" t="str">
-        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="75" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E75" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F75" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F75" s="15" t="str">
-        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="76" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E76" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F76" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F76" s="15" t="str">
-        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="77" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E77" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F77" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F77" s="15" t="str">
-        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="78" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E78" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F78" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F78" s="15" t="str">
-        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="79" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E79" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F79" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F79" s="15" t="str">
-        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="80" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E80" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F80" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F80" s="15" t="str">
-        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="81" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E81" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F81" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F81" s="15" t="str">
-        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="82" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E82" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F82" s="15" t="str">
-        <f t="shared" ref="F82:F121" si="8">IF(ISBLANK(A82),"",A82/(HOUR(E82) + MINUTE(E82) / 60))</f>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F82" s="14" t="str">
+        <f t="shared" ref="F82:F121" si="7">IF(ISBLANK(A82),"",A82/(HOUR(E82) + MINUTE(E82) / 60))</f>
         <v/>
       </c>
     </row>
     <row r="83" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E83" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F83" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F83" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="84" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E84" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F84" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F84" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="85" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E85" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F85" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F85" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="86" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E86" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F86" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F86" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="87" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E87" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F87" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F87" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="88" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E88" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F88" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F88" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="89" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E89" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F89" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F89" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="90" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E90" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F90" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F90" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="91" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E91" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F91" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F91" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="92" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E92" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F92" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F92" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="93" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E93" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F93" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F93" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="94" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E94" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F94" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F94" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="95" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E95" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F95" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F95" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="96" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E96" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F96" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F96" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="97" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E97" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F97" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F97" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="98" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E98" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F98" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F98" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="99" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E99" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F99" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F99" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="100" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E100" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F100" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F100" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="101" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E101" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F101" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F101" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="102" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E102" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F102" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F102" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="103" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E103" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F103" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F103" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="104" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E104" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F104" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F104" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="105" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E105" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F105" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F105" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="106" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E106" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F106" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F106" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="107" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E107" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F107" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F107" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="108" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E108" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F108" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F108" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="109" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E109" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F109" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F109" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="110" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E110" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F110" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F110" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="111" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E111" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F111" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F111" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="112" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E112" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F112" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F112" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="113" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E113" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F113" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F113" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="114" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E114" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F114" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F114" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="115" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E115" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F115" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F115" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="116" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E116" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F116" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F116" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="117" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E117" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F117" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F117" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="118" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E118" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F118" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F118" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="119" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E119" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F119" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F119" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="120" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E120" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F120" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F120" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="121" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E121" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F121" s="15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F121" s="14" t="str">
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="122" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E122" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="123" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E123" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="124" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E124" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="125" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E125" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="126" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E126" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="127" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E127" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="128" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E128" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="129" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E129" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="130" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E130" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="131" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E131" s="3" t="str">
-        <f t="shared" ref="E131:E151" si="9">IF(ISBLANK(D131),"",TEXT(D131-C131, "h:mm"))</f>
+        <f t="shared" ref="E131:E151" si="8">IF(ISBLANK(D131),"",TEXT(D131-C131, "h:mm"))</f>
         <v/>
       </c>
     </row>
     <row r="132" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E132" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="133" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E133" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="134" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E134" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="135" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E135" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="136" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E136" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="137" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E137" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="138" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E138" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="139" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E139" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="140" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E140" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="141" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E141" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="142" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E142" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="143" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E143" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="144" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E144" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="145" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E145" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="146" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E146" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="147" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E147" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="148" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E148" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="149" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E149" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="150" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E150" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="151" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E151" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>

</xml_diff>